<commit_message>
Input schem is just a pair of lists
</commit_message>
<xml_diff>
--- a/tests/fixtures/template.xlsx
+++ b/tests/fixtures/template.xlsx
@@ -29,7 +29,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Any string</t>
+          <t>Start of the alphabet</t>
         </r>
       </text>
     </comment>
@@ -42,33 +42,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Positive number</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>"A", "B", or "C"</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Only vowels are allowed</t>
+          <t>End of the alphabet</t>
         </r>
       </text>
     </comment>
@@ -77,13 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>a_string</t>
-  </si>
-  <si>
-    <t>positive</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>abc</t>
   </si>
@@ -97,7 +65,16 @@
     <t>C</t>
   </si>
   <si>
-    <t>only_vowels</t>
+    <t>xyz</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Z</t>
   </si>
 </sst>
 </file>
@@ -446,29 +423,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576">
+      <formula1>$'Value lists'.$A$1:$A$3</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576">
       <formula1>$'Value lists'.$A$1:$A$3</formula1>
     </dataValidation>
   </dataValidations>
@@ -487,17 +461,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rename temp file, regenerate excel fixture
</commit_message>
<xml_diff>
--- a/tests/fixtures/template.xlsx
+++ b/tests/fixtures/template.xlsx
@@ -8,7 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="Export this as TSV" sheetId="1" r:id="rId1"/>
-    <sheet name="Value lists" sheetId="2" r:id="rId2"/>
+    <sheet name="abc list" sheetId="2" r:id="rId2"/>
+    <sheet name="xyz list" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -440,10 +441,10 @@
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576">
-      <formula1>$'Value lists'.$A$1:$A$3</formula1>
+      <formula1>"A,B,C"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576">
-      <formula1>$'Value lists'.$A$1:$A$3</formula1>
+      <formula1>"X,Y,Z"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -461,6 +462,34 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Just enums and testing (#3)
* function factory to class factory; add second sheet

* Get subclassing right

* Tests pass locally

* Input schem is just a pair of lists

* pytest setup/teardown

* Parameterize test

* move comment

* Generate one sheet per enum. Tests broken, XLS broken

* expand readme

* Still not loading in Excel

* Fall back to old style to get it to work

* Rename temp file, regenerate excel fixture
</commit_message>
<xml_diff>
--- a/tests/fixtures/template.xlsx
+++ b/tests/fixtures/template.xlsx
@@ -7,7 +7,9 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Export this as TSV" sheetId="1" r:id="rId1"/>
+    <sheet name="abc list" sheetId="2" r:id="rId2"/>
+    <sheet name="xyz list" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -28,7 +30,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Any string</t>
+          <t>Start of the alphabet</t>
         </r>
       </text>
     </comment>
@@ -41,33 +43,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Positive number</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>"A", "B", or "C"</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Only vowels are allowed</t>
+          <t>End of the alphabet</t>
         </r>
       </text>
     </comment>
@@ -76,18 +52,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>a_string</t>
-  </si>
-  <si>
-    <t>positive</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>abc</t>
   </si>
   <si>
-    <t>only_vowels</t>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>xyz</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Z</t>
   </si>
 </sst>
 </file>
@@ -436,39 +424,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must be one of: A, B, C" sqref="C2:C1048576">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576">
       <formula1>"A,B,C"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
-      <formula1>A1="TODO"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576">
+      <formula1>"X,Y,Z"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
type constraints / packaging (#5)
* Create setup.py

* add twine

* full urls, so it works on pypi

* Rename package

* fix tests

* dependencies

* Build instructions in README

* Make package explicit

* Reference publish.sh

* switch to production pypi

* python version requirement too high

* Update README with pip

* Fix path problem with ts2xl

* Put JSON in Python, for simplicity

* Version bump

* Boolean validation

* Numeric type validation
</commit_message>
<xml_diff>
--- a/tests/fixtures/template.xlsx
+++ b/tests/fixtures/template.xlsx
@@ -47,12 +47,64 @@
         </r>
       </text>
     </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Any string</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Any number</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Any integer</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Any boolean</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>abc</t>
   </si>
@@ -76,6 +128,18 @@
   </si>
   <si>
     <t>Z</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>boolean</t>
   </si>
 </sst>
 </file>
@@ -424,27 +488,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576">
       <formula1>'abc list'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576">
       <formula1>'xyz list'!$A$1:$A$3</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
+      <formula1>-1e+307</formula1>
+      <formula2>1e+307</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576">
+      <formula1>-2147483647</formula1>
+      <formula2>2147483647</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576">
+      <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Freeze first row. Fix #14
</commit_message>
<xml_diff>
--- a/tests/fixtures/template.xlsx
+++ b/tests/fixtures/template.xlsx
@@ -490,7 +490,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>

</xml_diff>

<commit_message>
test handling of long enum names
</commit_message>
<xml_diff>
--- a/tests/fixtures/template.xlsx
+++ b/tests/fixtures/template.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Enter data here" sheetId="1" r:id="rId1"/>
     <sheet name="abc list" sheetId="2" r:id="rId2"/>
-    <sheet name="xyz list" sheetId="3" r:id="rId3"/>
+    <sheet name="xyz (Fields wi...t names.) list" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -118,7 +118,7 @@
     <t>C</t>
   </si>
   <si>
-    <t>xyz</t>
+    <t>xyz (Fields with enum constraints and names longer than 32 characters will have trucated sheet names.)</t>
   </si>
   <si>
     <t>X</t>
@@ -523,7 +523,7 @@
       <formula1>'abc list'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576">
-      <formula1>'xyz list'!$A$1:$A$3</formula1>
+      <formula1>'xyz (Fields wi...t names.) list'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>-1e+307</formula1>

</xml_diff>

<commit_message>
Make excel fixture less ugly: We have doctest
</commit_message>
<xml_diff>
--- a/tests/fixtures/template.xlsx
+++ b/tests/fixtures/template.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Enter data here" sheetId="1" r:id="rId1"/>
     <sheet name="abc list" sheetId="2" r:id="rId2"/>
-    <sheet name="xyz (Fields wi...t names.) list" sheetId="3" r:id="rId3"/>
+    <sheet name="xyz list" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -118,7 +118,7 @@
     <t>C</t>
   </si>
   <si>
-    <t>xyz (Fields with enum constraints and names longer than 32 characters will have trucated sheet names.)</t>
+    <t>xyz</t>
   </si>
   <si>
     <t>X</t>
@@ -523,7 +523,7 @@
       <formula1>'abc list'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576">
-      <formula1>'xyz (Fields wi...t names.) list'!$A$1:$A$3</formula1>
+      <formula1>'xyz list'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>-1e+307</formula1>

</xml_diff>

<commit_message>
row freeze / cli docs / schema validation down (#22)
* Freeze first row. Fix #14

* test handling of long enum names

* Make excel fixture less ugly: We have doctest

* Move validation down. Fix #13

* Checkin CLI help

* link from readme. Fix #16

* Make both versions happy
</commit_message>
<xml_diff>
--- a/tests/fixtures/template.xlsx
+++ b/tests/fixtures/template.xlsx
@@ -490,7 +490,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>

</xml_diff>

<commit_message>
Rename file for clarity; add constraints... but not processed
</commit_message>
<xml_diff>
--- a/tests/fixtures/template.xlsx
+++ b/tests/fixtures/template.xlsx
@@ -69,7 +69,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Any number</t>
+          <t>Any number &gt;= zero</t>
         </r>
       </text>
     </comment>
@@ -82,7 +82,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Any integer</t>
+          <t>An integer between 1 and 10</t>
         </r>
       </text>
     </comment>

</xml_diff>

<commit_message>
Numeric min and max... still need to update message
</commit_message>
<xml_diff>
--- a/tests/fixtures/template.xlsx
+++ b/tests/fixtures/template.xlsx
@@ -526,12 +526,12 @@
       <formula1>'xyz list'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="D2:D1048576">
-      <formula1>-1e+307</formula1>
+      <formula1>0</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not an integer" error="The values in this column must be integers." sqref="E2:E1048576">
-      <formula1>-2147483647</formula1>
-      <formula2>2147483647</formula2>
+      <formula1>1</formula1>
+      <formula2>10</formula2>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a boolean" error="The values in this column must be &quot;TRUE&quot; or &quot;FALSE&quot;." sqref="F2:F1048576">
       <formula1>"TRUE,FALSE"</formula1>

</xml_diff>

<commit_message>
Bounds checks on numbers
</commit_message>
<xml_diff>
--- a/tests/fixtures/template.xlsx
+++ b/tests/fixtures/template.xlsx
@@ -525,11 +525,11 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: X / Y / Z." sqref="B2:B1048576">
       <formula1>'xyz list'!$A$1:$A$3</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="D2:D1048576">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers &gt;= 0." sqref="D2:D1048576">
       <formula1>0</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not an integer" error="The values in this column must be integers." sqref="E2:E1048576">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not an integer" error="The values in this column must be integers between 1 and 10." sqref="E2:E1048576">
       <formula1>1</formula1>
       <formula2>10</formula2>
     </dataValidation>

</xml_diff>